<commit_message>
0.3.0 Support for Specifying Sheet Name
- Fleshed out my technique to dynamically instantiate dataclasses using ArgumentParser
- Fixed a bug where this wasn't actually working on the CLI because I didn't have __name__ == "__main__" at the bottom
-
</commit_message>
<xml_diff>
--- a/tests/_data/sample_wkbk.xlsx
+++ b/tests/_data/sample_wkbk.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sharedspace-my.sharepoint.com/personal/xavier_lian_wdc_com/Documents/Documents/OriginlessCode/xl-excel/tests/_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xavierlian/Documents/Code/xl-excel/tests/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{0373046F-D4FE-7644-9190-53DD799027EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9E4237B-DB7B-614C-8FBF-189BE26FA956}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6274D5-7B0C-384A-8B38-44B0E8853FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1320" windowWidth="27560" windowHeight="16940" xr2:uid="{E12BA67F-F063-3C4D-8D52-4B4515DD0A59}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>